<commit_message>
Udacity. final state after some corrections
</commit_message>
<xml_diff>
--- a/C1 - Azure Infrastructure Operations/Checkliste.xlsx
+++ b/C1 - Azure Infrastructure Operations/Checkliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wirch01\work\Projekte\Udacity\Cloud_DevOPS_Trac_2023\nd082-Azure-Cloud-DevOps-Starter-Code\C1 - Azure Infrastructure Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34BFFF39-BAFD-46C9-A270-07E8D35A34D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C510AE-280E-4BAC-B606-775E68D431AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{229632B3-ADF3-48E3-A1CD-9E7EB0FE079D}"/>
+    <workbookView xWindow="39060" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{229632B3-ADF3-48E3-A1CD-9E7EB0FE079D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Criteria</t>
   </si>
@@ -540,13 +540,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -611,6 +604,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -618,16 +617,17 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -643,12 +643,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E1DA42F-E9F0-4906-A080-9EF5FA9CB891}" name="Tabelle1" displayName="Tabelle1" ref="A1:C23" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E1DA42F-E9F0-4906-A080-9EF5FA9CB891}" name="Tabelle1" displayName="Tabelle1" ref="A1:C23" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:C23" xr:uid="{1E1DA42F-E9F0-4906-A080-9EF5FA9CB891}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{58F53084-3625-4FE6-BC2E-C978F0FDED15}" name="Criteria" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C8DE5DF0-D908-45E8-9CDF-3558A70623A0}" name="Meets Specifications" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{40F9080B-162F-40D6-A8E0-8EC1946D2046}" name="Checks" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{58F53084-3625-4FE6-BC2E-C978F0FDED15}" name="Criteria" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C8DE5DF0-D908-45E8-9CDF-3558A70623A0}" name="Meets Specifications" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{40F9080B-162F-40D6-A8E0-8EC1946D2046}" name="Checks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -954,7 +954,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="51.85546875" defaultRowHeight="15"/>
@@ -982,7 +982,9 @@
       <c r="B2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="75">
       <c r="A3" s="1" t="s">
@@ -991,7 +993,9 @@
       <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
@@ -1000,7 +1004,9 @@
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" s="1" t="s">
@@ -1009,7 +1015,9 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -1018,14 +1026,18 @@
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="30">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="30" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -1045,14 +1057,18 @@
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="30">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
@@ -1061,14 +1077,18 @@
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -1077,28 +1097,36 @@
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" s="1" t="s">
@@ -1107,7 +1135,9 @@
       <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
@@ -1116,14 +1146,18 @@
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="30">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="30">
       <c r="A20" s="1" t="s">
@@ -1132,14 +1166,18 @@
       <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="30">
       <c r="A22" s="1" t="s">
@@ -1148,7 +1186,9 @@
       <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="30">
       <c r="A23" s="1" t="s">
@@ -1157,7 +1197,9 @@
       <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
@@ -1170,7 +1212,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
     <cfRule type="iconSet" priority="3">

</xml_diff>